<commit_message>
Patched to Update Asset List Daily
This is in case over the long run an asset goes from ETB to HTB
</commit_message>
<xml_diff>
--- a/BackTestingShortie/Results/percent_returns.xlsx
+++ b/BackTestingShortie/Results/percent_returns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aidanjalili03/Desktop/Edison/BackTestingShortie/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF390D38-6755-3C42-AE27-3E2BA4F5B617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8575F121-A2B9-6141-8AA3-555091B91091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15475,8 +15475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L1019"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A786" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15532,8 +15532,8 @@
         <v>318</v>
       </c>
       <c r="L2">
-        <f>COUNTIF(C:C,"&gt;0")</f>
-        <v>804</v>
+        <f>COUNTIF(G:G,"&gt;0")</f>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -15569,8 +15569,8 @@
         <v>317</v>
       </c>
       <c r="L3">
-        <f>COUNTIF(C:C,"&lt;0")</f>
-        <v>214</v>
+        <f>COUNTIF(G:G,"&lt;0")</f>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -15637,7 +15637,7 @@
       </c>
       <c r="L5">
         <f>L2/L3</f>
-        <v>3.7570093457943927</v>
+        <v>0.52066115702479343</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>